<commit_message>
dont with excel now i think
</commit_message>
<xml_diff>
--- a/thesis-graphs.xlsx
+++ b/thesis-graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\thesis\thesis-report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED31354D-971A-4592-901B-25B210AB5349}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A422DDF-E0A6-4885-923C-9E69B8470A1C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>64 byte comparison</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>ntop</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>%loss</t>
+  </si>
+  <si>
+    <t>GRAPHICAL REPRESENTATIONS OF OTHER FRAMEWORKS ARE NOT VERY INTERESTING</t>
   </si>
 </sst>
 </file>
@@ -8169,15 +8181,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>440531</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>526256</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8240,16 +8252,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>488157</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>11906</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>23814</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>280987</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>135732</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8682,10 +8694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ162"/>
+  <dimension ref="A1:AMJ204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U71" sqref="U71"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J165" sqref="J165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10737,7 +10749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="6:10">
+    <row r="161" spans="4:18">
       <c r="F161">
         <v>1155</v>
       </c>
@@ -10753,7 +10765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="6:10">
+    <row r="162" spans="4:18">
       <c r="F162">
         <v>583</v>
       </c>
@@ -10766,6 +10778,467 @@
       </c>
       <c r="J162">
         <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="4:18">
+      <c r="D171" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="174" spans="4:18">
+      <c r="I174">
+        <v>64</v>
+      </c>
+      <c r="K174">
+        <v>128</v>
+      </c>
+      <c r="M174">
+        <v>256</v>
+      </c>
+      <c r="O174">
+        <v>512</v>
+      </c>
+      <c r="Q174">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="175" spans="4:18">
+      <c r="D175" t="s">
+        <v>11</v>
+      </c>
+      <c r="E175" t="s">
+        <v>12</v>
+      </c>
+      <c r="F175" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="176" spans="4:18">
+      <c r="D176">
+        <v>0.1</v>
+      </c>
+      <c r="E176">
+        <v>64</v>
+      </c>
+      <c r="F176">
+        <v>0</v>
+      </c>
+      <c r="I176" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="J176" s="9">
+        <v>0</v>
+      </c>
+      <c r="K176" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="L176" s="9">
+        <v>0</v>
+      </c>
+      <c r="M176" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="N176" s="9">
+        <v>0</v>
+      </c>
+      <c r="O176" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="P176" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q176" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="R176" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="4:18">
+      <c r="D177">
+        <v>0.1</v>
+      </c>
+      <c r="E177">
+        <v>128</v>
+      </c>
+      <c r="F177">
+        <v>0</v>
+      </c>
+      <c r="I177" s="9">
+        <v>1</v>
+      </c>
+      <c r="J177" s="9">
+        <v>0</v>
+      </c>
+      <c r="K177" s="9">
+        <v>1</v>
+      </c>
+      <c r="L177" s="9">
+        <v>0</v>
+      </c>
+      <c r="M177" s="9">
+        <v>1</v>
+      </c>
+      <c r="N177" s="9">
+        <v>0</v>
+      </c>
+      <c r="O177" s="9">
+        <v>1</v>
+      </c>
+      <c r="P177" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q177" s="9">
+        <v>1</v>
+      </c>
+      <c r="R177" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="4:18">
+      <c r="D178">
+        <v>0.1</v>
+      </c>
+      <c r="E178">
+        <v>256</v>
+      </c>
+      <c r="F178">
+        <v>0</v>
+      </c>
+      <c r="I178" s="9">
+        <v>5</v>
+      </c>
+      <c r="J178" s="9">
+        <v>7.7356031999999991E-2</v>
+      </c>
+      <c r="K178" s="9">
+        <v>5</v>
+      </c>
+      <c r="L178" s="9">
+        <v>0</v>
+      </c>
+      <c r="M178" s="9">
+        <v>5</v>
+      </c>
+      <c r="N178" s="9">
+        <v>0</v>
+      </c>
+      <c r="O178" s="9">
+        <v>5</v>
+      </c>
+      <c r="P178" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q178" s="9">
+        <v>5</v>
+      </c>
+      <c r="R178" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="4:18">
+      <c r="D179">
+        <v>0.1</v>
+      </c>
+      <c r="E179">
+        <v>512</v>
+      </c>
+      <c r="F179">
+        <v>0</v>
+      </c>
+      <c r="I179" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="J179" s="9">
+        <v>0.12223146666666668</v>
+      </c>
+      <c r="K179" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="L179" s="9">
+        <v>2.7821397143405931E-2</v>
+      </c>
+      <c r="M179" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="N179" s="9">
+        <v>0</v>
+      </c>
+      <c r="O179" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="P179" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q179" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="R179" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="4:18">
+      <c r="D180">
+        <v>0.1</v>
+      </c>
+      <c r="E180">
+        <v>1024</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+      <c r="I180" s="9">
+        <v>10</v>
+      </c>
+      <c r="J180" s="9">
+        <v>4.5735362559999997</v>
+      </c>
+      <c r="K180" s="9">
+        <v>10</v>
+      </c>
+      <c r="L180" s="9">
+        <v>9.958297599999999E-2</v>
+      </c>
+      <c r="M180" s="9">
+        <v>10</v>
+      </c>
+      <c r="N180" s="9">
+        <v>0</v>
+      </c>
+      <c r="O180" s="9">
+        <v>10</v>
+      </c>
+      <c r="P180" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q180" s="9">
+        <v>10</v>
+      </c>
+      <c r="R180" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="4:18">
+      <c r="R181" s="9"/>
+    </row>
+    <row r="182" spans="4:18">
+      <c r="D182">
+        <v>1</v>
+      </c>
+      <c r="E182">
+        <v>64</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="4:18">
+      <c r="D183">
+        <v>1</v>
+      </c>
+      <c r="E183">
+        <v>128</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="4:18">
+      <c r="D184">
+        <v>1</v>
+      </c>
+      <c r="E184">
+        <v>256</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="4:18">
+      <c r="D185">
+        <v>1</v>
+      </c>
+      <c r="E185">
+        <v>512</v>
+      </c>
+      <c r="F185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="4:18">
+      <c r="D186">
+        <v>1</v>
+      </c>
+      <c r="E186">
+        <v>1024</v>
+      </c>
+      <c r="F186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="4:18">
+      <c r="D188">
+        <v>5</v>
+      </c>
+      <c r="E188">
+        <v>64</v>
+      </c>
+      <c r="F188">
+        <v>7.7356031999999991E-2</v>
+      </c>
+    </row>
+    <row r="189" spans="4:18">
+      <c r="D189">
+        <v>5</v>
+      </c>
+      <c r="E189">
+        <v>128</v>
+      </c>
+      <c r="F189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="4:18">
+      <c r="D190">
+        <v>5</v>
+      </c>
+      <c r="E190">
+        <v>256</v>
+      </c>
+      <c r="F190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="4:18">
+      <c r="D191">
+        <v>5</v>
+      </c>
+      <c r="E191">
+        <v>512</v>
+      </c>
+      <c r="F191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="4:18">
+      <c r="D192">
+        <v>5</v>
+      </c>
+      <c r="E192">
+        <v>1024</v>
+      </c>
+      <c r="F192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="4:6">
+      <c r="D194">
+        <v>7.5</v>
+      </c>
+      <c r="E194">
+        <v>64</v>
+      </c>
+      <c r="F194">
+        <v>0.12223146666666668</v>
+      </c>
+    </row>
+    <row r="195" spans="4:6">
+      <c r="D195">
+        <v>7.5</v>
+      </c>
+      <c r="E195">
+        <v>128</v>
+      </c>
+      <c r="F195">
+        <v>2.7821397143405931E-2</v>
+      </c>
+    </row>
+    <row r="196" spans="4:6">
+      <c r="D196">
+        <v>7.5</v>
+      </c>
+      <c r="E196">
+        <v>256</v>
+      </c>
+      <c r="F196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="4:6">
+      <c r="D197">
+        <v>7.5</v>
+      </c>
+      <c r="E197">
+        <v>512</v>
+      </c>
+      <c r="F197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="4:6">
+      <c r="D198">
+        <v>7.5</v>
+      </c>
+      <c r="E198">
+        <v>1024</v>
+      </c>
+      <c r="F198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="4:6">
+      <c r="D200">
+        <v>10</v>
+      </c>
+      <c r="E200">
+        <v>64</v>
+      </c>
+      <c r="F200">
+        <v>4.5735362559999997</v>
+      </c>
+    </row>
+    <row r="201" spans="4:6">
+      <c r="D201">
+        <v>10</v>
+      </c>
+      <c r="E201">
+        <v>128</v>
+      </c>
+      <c r="F201">
+        <v>9.958297599999999E-2</v>
+      </c>
+    </row>
+    <row r="202" spans="4:6">
+      <c r="D202">
+        <v>10</v>
+      </c>
+      <c r="E202">
+        <v>256</v>
+      </c>
+      <c r="F202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="4:6">
+      <c r="D203">
+        <v>10</v>
+      </c>
+      <c r="E203">
+        <v>512</v>
+      </c>
+      <c r="F203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="4:6">
+      <c r="D204">
+        <v>10</v>
+      </c>
+      <c r="E204">
+        <v>1024</v>
+      </c>
+      <c r="F204">
         <v>0</v>
       </c>
     </row>

</xml_diff>